<commit_message>
Add shopping cart "basket" functionality, tested in swagger
</commit_message>
<xml_diff>
--- a/Microservices/src/API_documentation.xlsx
+++ b/Microservices/src/API_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\WEBSITE_PROJECTS\_TUTORIALS\microservices\Microservices\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8795DC04-130B-4C6A-82FB-4AFB6EB521BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863CDAB2-9DB3-4DDB-835C-A6556BFA9798}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17595" yWindow="4448" windowWidth="21600" windowHeight="11422" xr2:uid="{492481FA-45E9-412F-BBEC-E1E54DF07088}"/>
+    <workbookView xWindow="7200" yWindow="3000" windowWidth="21600" windowHeight="11423" xr2:uid="{492481FA-45E9-412F-BBEC-E1E54DF07088}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Method</t>
   </si>
@@ -88,6 +88,30 @@
   </si>
   <si>
     <t>Catalog</t>
+  </si>
+  <si>
+    <t>Basket</t>
+  </si>
+  <si>
+    <t>api/vi/Basket</t>
+  </si>
+  <si>
+    <t>Get Basket and Items with Username</t>
+  </si>
+  <si>
+    <t>api/vi/Basket/{id}</t>
+  </si>
+  <si>
+    <t>api/vi/Basket/Checkout</t>
+  </si>
+  <si>
+    <t>Checkout Basket</t>
+  </si>
+  <si>
+    <t>Delete Basket</t>
+  </si>
+  <si>
+    <t>Update Basket and Items (add - remove item on basket)</t>
   </si>
 </sst>
 </file>
@@ -143,8 +167,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37A37F3E-FA0A-4CB0-95BB-19DE73BD8832}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7" xr:uid="{2F633495-9DF3-423A-AF4A-188D0F75928A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{37A37F3E-FA0A-4CB0-95BB-19DE73BD8832}" name="Table1" displayName="Table1" ref="A1:D20" totalsRowShown="0">
+  <autoFilter ref="A1:D20" xr:uid="{2F633495-9DF3-423A-AF4A-188D0F75928A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{287FB3FF-BD1B-4B47-8551-4FF0F6665C9C}" name="API"/>
     <tableColumn id="2" xr3:uid="{BDB440A2-4831-410D-A3A3-E5786CBB9C43}" name="Method"/>
@@ -452,17 +476,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E13AFD-F2EB-458F-8174-60E460661621}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D7"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="10.59765625" customWidth="1"/>
     <col min="3" max="3" width="40.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
@@ -561,6 +585,62 @@
       </c>
       <c r="D7" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and tested rabbitmq module, dockerized it and basket
</commit_message>
<xml_diff>
--- a/Microservices/src/API_documentation.xlsx
+++ b/Microservices/src/API_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\WEBSITE_PROJECTS\_TUTORIALS\microservices\Microservices\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863CDAB2-9DB3-4DDB-835C-A6556BFA9798}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2506F6F6-1520-403D-9F46-3ED963DAFB83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3000" windowWidth="21600" windowHeight="11423" xr2:uid="{492481FA-45E9-412F-BBEC-E1E54DF07088}"/>
+    <workbookView xWindow="338" yWindow="3278" windowWidth="21600" windowHeight="11422" xr2:uid="{492481FA-45E9-412F-BBEC-E1E54DF07088}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Method</t>
   </si>
@@ -93,18 +93,9 @@
     <t>Basket</t>
   </si>
   <si>
-    <t>api/vi/Basket</t>
-  </si>
-  <si>
     <t>Get Basket and Items with Username</t>
   </si>
   <si>
-    <t>api/vi/Basket/{id}</t>
-  </si>
-  <si>
-    <t>api/vi/Basket/Checkout</t>
-  </si>
-  <si>
     <t>Checkout Basket</t>
   </si>
   <si>
@@ -112,6 +103,30 @@
   </si>
   <si>
     <t>Update Basket and Items (add - remove item on basket)</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>api/v1/Order</t>
+  </si>
+  <si>
+    <t>Get Orders with username</t>
+  </si>
+  <si>
+    <t>api/v1/Basket</t>
+  </si>
+  <si>
+    <t>api/v1/Basket/{id}</t>
+  </si>
+  <si>
+    <t>api/v1/Basket/Checkout</t>
+  </si>
+  <si>
+    <t>Post Orders with username (for testing)</t>
+  </si>
+  <si>
+    <t>api/v1/Order/</t>
   </si>
 </sst>
 </file>
@@ -476,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E13AFD-F2EB-458F-8174-60E460661621}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -595,10 +610,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -609,10 +624,10 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -623,10 +638,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
         <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -637,10 +652,38 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>